<commit_message>
update read excel data
</commit_message>
<xml_diff>
--- a/PalindromeCheckerTest_06_Khang/TestData/TestData.xlsx
+++ b/PalindromeCheckerTest_06_Khang/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
     <x:t>ExpectedOutput</x:t>
   </x:si>
   <x:si>
-    <x:t>madam</x:t>
+    <x:t>66x66</x:t>
   </x:si>
   <x:si>
     <x:t>True</x:t>
@@ -437,7 +437,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
@@ -453,7 +453,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>